<commit_message>
task 4 in progress...
</commit_message>
<xml_diff>
--- a/1. Basics/task_4/condition_combinations_4.xlsx
+++ b/1. Basics/task_4/condition_combinations_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\~УЧЕБА\~ПРОГРАМУВАННЯ\~PHP\Нова папка\1. Basics\task__4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\~УЧЕБА\~ПРОГРАМУВАННЯ\~PHP\2. SH++\1. Basics\task_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5781DD6B-6644-4E75-AA6A-E6BA4CBD7DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B624BF20-F72F-4D8C-9B01-72BF52306FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="67">
   <si>
     <t>method</t>
   </si>
@@ -197,12 +197,6 @@
     <t>not POST</t>
   </si>
   <si>
-    <t>&lt;h1 style="color:red"&gt;NOT FOUND&lt;/h1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h1 style="color:red"&gt;SMTH WRONG. CONTACT TO YOUR ADMIN&lt;/h1&gt;</t>
-  </si>
-  <si>
     <t>немає через криве body</t>
   </si>
   <si>
@@ -222,6 +216,18 @@
   </si>
   <si>
     <t>406, 422</t>
+  </si>
+  <si>
+    <t>Unprocessable Entity</t>
+  </si>
+  <si>
+    <t>&lt;h1 style="color:red"&gt;Not Found&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;Bad Request&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;Internal Server Error&lt;/h1&gt;</t>
   </si>
 </sst>
 </file>
@@ -258,18 +264,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -314,23 +314,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -669,37 +669,37 @@
       <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>200</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -707,37 +707,37 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>404</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -745,35 +745,35 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>400</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -781,35 +781,35 @@
       <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>400</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -828,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -1018,57 +1018,57 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:3">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="3:3">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="3:3">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="3:3">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="3:3">
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="3:3">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="3:3">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="3:3">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="3:3">
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B1A18B-CB39-4375-B6D4-5EF6A2BC4A76}">
   <dimension ref="A3:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1180,14 +1180,14 @@
       <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="5">
-        <v>400</v>
+      <c r="I5" s="11">
+        <v>404</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1210,16 +1210,16 @@
         <v>49</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="5">
+        <v>56</v>
+      </c>
+      <c r="I6" s="11">
         <v>400</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1235,12 +1235,12 @@
       <c r="J7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>25</v>
+      <c r="K7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>1.1000000000000001</v>
       </c>
       <c r="C8" t="s">
@@ -1252,12 +1252,12 @@
       <c r="J8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>25</v>
+      <c r="K8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>2</v>
       </c>
       <c r="D9" t="s">
@@ -1269,12 +1269,12 @@
       <c r="J9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>25</v>
+      <c r="K9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>1.2</v>
       </c>
       <c r="E10" t="s">
@@ -1286,8 +1286,8 @@
       <c r="J10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>25</v>
+      <c r="K10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1295,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1303,13 +1303,13 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1317,49 +1317,60 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:9">
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="4:6">
+        <v>59</v>
+      </c>
+      <c r="F17" s="3">
+        <v>422</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9">
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6">
+        <v>60</v>
+      </c>
+      <c r="F18" s="3">
+        <v>403</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9">
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9">
       <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9">
       <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>